<commit_message>
adding row onto meat file
</commit_message>
<xml_diff>
--- a/food_groups/meat.xlsx
+++ b/food_groups/meat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34B27729-193E-4E61-A184-EB3DF79F98E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622E3D79-4B06-4002-AEA3-1896EF4BEBFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meat" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Lamb</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F63B581-3CCF-406A-BC79-D32FBF339614}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A22"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,39 +490,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -524,17 +530,25 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="b">
+      <c r="B8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -545,10 +559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,41 +574,49 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -605,10 +627,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AE204F-D8BB-49D6-9E4D-47532BCE6A6E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,17 +641,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -640,10 +670,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7422A70D-287B-44C2-AE10-BFA854CED454}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,17 +684,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -675,10 +713,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356DD906-8FAA-4118-9BEC-32AEDD4E9133}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,41 +730,49 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -737,42 +783,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D150B1A3-CAB0-4845-BCE5-1361B698E08E}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34029E5-578B-4625-9CCF-B17AA8D2F971}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,17 +796,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -801,12 +823,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3FDBF9-13FB-4B8C-AE3D-F0C9FB2A2108}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34029E5-578B-4625-9CCF-B17AA8D2F971}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,17 +838,67 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3FDBF9-13FB-4B8C-AE3D-F0C9FB2A2108}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setting up vegetarian sub
</commit_message>
<xml_diff>
--- a/food_groups/meat.xlsx
+++ b/food_groups/meat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5652DA6-EE5C-4BAB-8100-CE5BB0C5BEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C593AB33-DAD5-4363-9C3C-C903A6FB7E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meat" sheetId="2" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="quail" sheetId="14" r:id="rId9"/>
     <sheet name="pheasant" sheetId="16" r:id="rId10"/>
     <sheet name="red meat" sheetId="3" r:id="rId11"/>
-    <sheet name="pork" sheetId="6" r:id="rId12"/>
-    <sheet name="goat" sheetId="18" r:id="rId13"/>
-    <sheet name="beef" sheetId="7" r:id="rId14"/>
-    <sheet name="lamb" sheetId="8" r:id="rId15"/>
-    <sheet name="bison" sheetId="13" r:id="rId16"/>
-    <sheet name="venison" sheetId="15" r:id="rId17"/>
-    <sheet name="rabbit" sheetId="17" r:id="rId18"/>
+    <sheet name="broth" sheetId="19" r:id="rId12"/>
+    <sheet name="pork" sheetId="6" r:id="rId13"/>
+    <sheet name="goat" sheetId="18" r:id="rId14"/>
+    <sheet name="beef" sheetId="7" r:id="rId15"/>
+    <sheet name="lamb" sheetId="8" r:id="rId16"/>
+    <sheet name="bison" sheetId="13" r:id="rId17"/>
+    <sheet name="venison" sheetId="15" r:id="rId18"/>
+    <sheet name="rabbit" sheetId="17" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="44">
   <si>
     <t>pass</t>
   </si>
@@ -173,6 +174,12 @@
   </si>
   <si>
     <t>goat</t>
+  </si>
+  <si>
+    <t>broth</t>
+  </si>
+  <si>
+    <t>vegetable broth</t>
   </si>
 </sst>
 </file>
@@ -527,7 +534,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356DD906-8FAA-4118-9BEC-32AEDD4E9133}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -759,6 +766,61 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAAD70A-5E0E-45B9-8577-A97E04C328E3}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D150B1A3-CAB0-4845-BCE5-1361B698E08E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -808,7 +870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82B3DA3-5D32-46C7-ADC1-5BEF79DD049F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -855,7 +917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34029E5-578B-4625-9CCF-B17AA8D2F971}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -905,7 +967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3FDBF9-13FB-4B8C-AE3D-F0C9FB2A2108}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -955,7 +1017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526732A-560E-44C0-B50C-EC6D45C50B1A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1002,7 +1064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DCE161-51E4-4C0F-A401-832F3D66E7C7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1049,7 +1111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA552B17-5FC0-42D9-A6CC-7A16AA0BE166}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
added healthy substitute for plant based meats
</commit_message>
<xml_diff>
--- a/food_groups/meat.xlsx
+++ b/food_groups/meat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0046085-B7B7-4BF7-88DC-693264A92266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E84BB9-AF70-42EF-A361-EF1C8BFAC8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="6" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meat" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="46">
   <si>
     <t>pass</t>
   </si>
@@ -828,10 +828,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D150B1A3-CAB0-4845-BCE5-1361B698E08E}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,6 +879,14 @@
         <v>44</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -941,10 +949,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34029E5-578B-4625-9CCF-B17AA8D2F971}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,6 +1000,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1169,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA552B17-5FC0-42D9-A6CC-7A16AA0BE166}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>